<commit_message>
[doc] Add explained features
- complete excel folder
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\FMI\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E7FB5-9152-44B8-BE92-7F264C67AEA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D976CE5E-76EA-495B-9CDB-66C11BAD143C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12255" yWindow="1875" windowWidth="21600" windowHeight="12540" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1875" windowWidth="21600" windowHeight="12540" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve">Author Name: </t>
   </si>
   <si>
-    <t>Popescu Ionel</t>
-  </si>
-  <si>
     <t>Georgescu Anca</t>
   </si>
   <si>
@@ -181,6 +178,69 @@
   </si>
   <si>
     <t>total sold is not computed</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>relationships are not named properly</t>
+  </si>
+  <si>
+    <t>Yes, the arhitecture accounts for all the requirements</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>No, errors are not handle</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>MenuRepository:42</t>
+  </si>
+  <si>
+    <t>double conversion can throw exception</t>
+  </si>
+  <si>
+    <t>PizzaService:32-37</t>
+  </si>
+  <si>
+    <t>Confuzion in use of variables</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>No, PizzaService is PaymentService</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>OrdersGuiController</t>
+  </si>
+  <si>
+    <t>* Disable payOrder until order is processed                         * Remove 0 from quantities</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>when client(cook) click on Ready without selecting an order will throw error</t>
+  </si>
+  <si>
+    <t>30min</t>
   </si>
 </sst>
 </file>
@@ -388,8 +448,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,10 +494,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,8 +837,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+    <sheetView topLeftCell="A2" zoomScale="120" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,33 +859,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -835,15 +895,15 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="24"/>
+      <c r="D4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="26"/>
       <c r="H4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -853,15 +913,15 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="26"/>
+      <c r="D5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="H5" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -872,15 +932,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -901,13 +961,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -916,13 +976,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1">
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -931,13 +991,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -946,13 +1006,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -961,13 +1021,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -976,13 +1036,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1083,7 +1143,9 @@
         <v>8</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1106,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,33 +1188,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1162,15 +1224,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="D4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="H4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1180,15 +1242,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="D5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="31"/>
       <c r="H5" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1199,15 +1261,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1223,40 +1285,56 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1406,8 +1484,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,8 +1493,8 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1427,33 +1505,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1463,15 +1541,15 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="D4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1481,15 +1559,15 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="32"/>
+      <c r="D5" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1500,15 +1578,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1528,36 +1606,58 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1720,7 +1820,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1766,33 +1868,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1800,15 +1902,15 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+        <v>24</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1818,13 +1920,13 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1835,24 +1937,24 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,11 +2170,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="C32" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[feat] Solve Sonar List warnings
- complete excel for sonar part
- solve warnings from Sonar
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\FMI\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0995747A-A14B-49FF-AB5B-7FA82722DBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE09C303-AD41-4B32-AE66-B0FE7C7DFA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21570" yWindow="2895" windowWidth="12900" windowHeight="12540" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="108">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -244,13 +244,124 @@
   </si>
   <si>
     <t>1h30min</t>
+  </si>
+  <si>
+    <t>Loop while true never end</t>
+  </si>
+  <si>
+    <t>KitchenGuiController:32</t>
+  </si>
+  <si>
+    <t>Remove loop</t>
+  </si>
+  <si>
+    <t>Make this anonymous inner class a lambda</t>
+  </si>
+  <si>
+    <t>Add stop condition to loop</t>
+  </si>
+  <si>
+    <t>new Runnable()</t>
+  </si>
+  <si>
+    <t>Replace with lambda</t>
+  </si>
+  <si>
+    <t>Remove this "String" constructor</t>
+  </si>
+  <si>
+    <t>KitchenGuiController:26</t>
+  </si>
+  <si>
+    <t>new String()</t>
+  </si>
+  <si>
+    <t>Replace with empty string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replace this use of System.out or System.err by a logger. </t>
+  </si>
+  <si>
+    <t>System.out.println</t>
+  </si>
+  <si>
+    <t>Log.print()</t>
+  </si>
+  <si>
+    <t>KitchenGuiController:64_66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make this "public static order" field final </t>
+  </si>
+  <si>
+    <t>public static</t>
+  </si>
+  <si>
+    <t>public static final</t>
+  </si>
+  <si>
+    <t>KitchenGuiController:23</t>
+  </si>
+  <si>
+    <t>Make this field protected</t>
+  </si>
+  <si>
+    <t>protected static final</t>
+  </si>
+  <si>
+    <t>Add a nested comment explaining why this method is empty</t>
+  </si>
+  <si>
+    <t>MainGUIController:47</t>
+  </si>
+  <si>
+    <t>Empty Constructor</t>
+  </si>
+  <si>
+    <t>Remove constructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Change this instance-reference to a static reference</t>
+  </si>
+  <si>
+    <t>OrdersGUIController:54</t>
+  </si>
+  <si>
+    <t>Was instance invocation</t>
+  </si>
+  <si>
+    <t>Class invocation</t>
+  </si>
+  <si>
+    <t>Rename this method to prevent any misunderstanding or make it a constructor</t>
+  </si>
+  <si>
+    <t>KitchenGUI:17</t>
+  </si>
+  <si>
+    <t>Method named like class</t>
+  </si>
+  <si>
+    <t>changed method name</t>
+  </si>
+  <si>
+    <t>Use try-with-resources or close this "BufferedReader" in a "finally" clause</t>
+  </si>
+  <si>
+    <t>MenuRepository:22</t>
+  </si>
+  <si>
+    <t>try with resources</t>
+  </si>
+  <si>
+    <t>try without resource closing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +431,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="5">
@@ -421,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,6 +615,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,7 +1293,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1850,17 +1972,17 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="6"/>
     <col min="8" max="8" width="12.28515625" style="6" customWidth="1"/>
@@ -1966,100 +2088,180 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">

</xml_diff>

<commit_message>
[refactor] Change misspelling words
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\FMI\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE09C303-AD41-4B32-AE66-B0FE7C7DFA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6117F4D-6599-4DE2-B2CB-88318FC08304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21570" yWindow="2895" windowWidth="12900" windowHeight="12540" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="107">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -66,12 +66,6 @@
     <t xml:space="preserve">Author Name: </t>
   </si>
   <si>
-    <t>Georgescu Anca</t>
-  </si>
-  <si>
-    <t>Firicescu George</t>
-  </si>
-  <si>
     <t>Requirements Document</t>
   </si>
   <si>
@@ -189,27 +183,18 @@
     <t>2h</t>
   </si>
   <si>
-    <t>relationships are not named properly</t>
-  </si>
-  <si>
     <t>Yes, the arhitecture accounts for all the requirements</t>
   </si>
   <si>
     <t>A05</t>
   </si>
   <si>
-    <t>No, errors are not handle</t>
-  </si>
-  <si>
     <t>C06</t>
   </si>
   <si>
     <t>MenuRepository:42</t>
   </si>
   <si>
-    <t>double conversion can throw exception</t>
-  </si>
-  <si>
     <t>PizzaService:32-37</t>
   </si>
   <si>
@@ -237,9 +222,6 @@
     <t>C07</t>
   </si>
   <si>
-    <t>when client(cook) click on Ready without selecting an order will throw error</t>
-  </si>
-  <si>
     <t>30min</t>
   </si>
   <si>
@@ -355,6 +337,21 @@
   </si>
   <si>
     <t>try without resource closing</t>
+  </si>
+  <si>
+    <t>Forgacs    Amelia</t>
+  </si>
+  <si>
+    <t>Relationships are not named properly</t>
+  </si>
+  <si>
+    <t>No, errors are not handled</t>
+  </si>
+  <si>
+    <t>When client(cook) click on Ready without selecting an order will throw error</t>
+  </si>
+  <si>
+    <t>Double conversion can throw exception</t>
   </si>
 </sst>
 </file>
@@ -540,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -571,6 +568,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -616,8 +616,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,7 +963,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,33 +984,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="H1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1020,15 +1020,15 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="26"/>
+      <c r="D4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="27"/>
       <c r="H4" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1038,15 +1038,15 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="28"/>
+      <c r="D5" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="H5" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1057,15 +1057,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="38">
+        <v>43887</v>
+      </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1086,13 +1088,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1101,13 +1103,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1">
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1116,13 +1118,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1131,13 +1133,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1146,13 +1148,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1161,13 +1163,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1269,7 +1271,7 @@
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1293,8 +1295,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,33 +1315,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="H1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1349,15 +1351,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="29"/>
+      <c r="D4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="30"/>
       <c r="H4" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1367,15 +1369,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="31"/>
+      <c r="D5" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="32"/>
       <c r="H5" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1386,15 +1388,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="38">
+        <v>43887</v>
+      </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1415,11 +1419,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,11 +1432,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1441,11 +1445,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1454,11 +1458,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1587,7 +1591,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1611,8 +1615,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,33 +1636,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="H1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -1668,15 +1672,15 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="32"/>
+      <c r="D4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1686,15 +1690,15 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="34"/>
+      <c r="D5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="35"/>
       <c r="H5" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1705,15 +1709,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="38">
+        <v>43887</v>
+      </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1734,13 +1740,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1749,11 +1755,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1762,13 +1768,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1777,13 +1783,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1948,7 +1954,7 @@
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1972,8 +1978,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,33 +2001,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="H1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="18">
         <v>233</v>
@@ -2029,15 +2035,15 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -2047,13 +2053,15 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="23"/>
       <c r="H5" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -2064,24 +2072,26 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="38">
+        <v>43887</v>
+      </c>
+      <c r="E6" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2089,16 +2099,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2107,16 +2117,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2125,16 +2135,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2143,16 +2153,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2161,16 +2171,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2179,16 +2189,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2197,16 +2207,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2215,16 +2225,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2232,17 +2242,17 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>101</v>
+      <c r="C18" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2251,16 +2261,16 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2377,11 +2387,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="C32" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[doc] Add Test Cases for project
- add xslx for ECP and BVC
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\FMI\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6117F4D-6599-4DE2-B2CB-88318FC08304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D82EEA3-5743-4496-B593-3FE09E70379A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -571,6 +571,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -615,9 +618,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,7 +962,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
@@ -984,19 +984,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>27</v>
@@ -1020,10 +1020,10 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="18" t="s">
         <v>18</v>
       </c>
@@ -1038,10 +1038,10 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="18" t="s">
         <v>19</v>
       </c>
@@ -1057,17 +1057,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="23">
         <v>43887</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1315,19 +1315,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>27</v>
@@ -1351,10 +1351,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="18" t="s">
         <v>18</v>
       </c>
@@ -1369,10 +1369,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="18" t="s">
         <v>19</v>
       </c>
@@ -1388,17 +1388,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="23">
         <v>43887</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1636,19 +1636,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>27</v>
@@ -1672,10 +1672,10 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>18</v>
       </c>
@@ -1690,10 +1690,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="18" t="s">
         <v>19</v>
       </c>
@@ -1709,17 +1709,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="23">
         <v>43887</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1978,7 +1978,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
@@ -2001,19 +2001,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>27</v>
@@ -2037,8 +2037,8 @@
       <c r="C4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>18</v>
       </c>
@@ -2053,10 +2053,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="18" t="s">
         <v>19</v>
       </c>
@@ -2072,10 +2072,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="23">
         <v>43887</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -2387,11 +2387,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>